<commit_message>
DS brandname: add column {DisplayTenantName}
</commit_message>
<xml_diff>
--- a/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ExcelTemplate/Brandname_Export_Template.xlsx
+++ b/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ExcelTemplate/Brandname_Export_Template.xlsx
@@ -32,28 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>HoTen</t>
-  </si>
-  <si>
-    <t>NgaySinh</t>
-  </si>
-  <si>
-    <t>SoDienThoai</t>
-  </si>
-  <si>
-    <t>CanCuocCongDan</t>
-  </si>
-  <si>
-    <t>TenTinhThanh</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>NgayBatDauLamViec</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Tên brandname</t>
   </si>
@@ -74,6 +53,9 @@
   </si>
   <si>
     <t>DANH SÁCH BRANDNAME</t>
+  </si>
+  <si>
+    <t>Tên cửa hàng</t>
   </si>
 </sst>
 </file>
@@ -524,212 +506,236 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CK13"/>
+  <dimension ref="A1:CL12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="16" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="24" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="16" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" style="16" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="24" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:90" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:90" x14ac:dyDescent="0.25">
+      <c r="L2" s="6"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="7"/>
+      <c r="AI2" s="7"/>
+      <c r="AJ2" s="7"/>
+      <c r="AK2" s="7"/>
+      <c r="AL2" s="7"/>
+      <c r="AM2" s="7"/>
+      <c r="AN2" s="7"/>
+      <c r="AO2" s="7"/>
+      <c r="AP2" s="7"/>
+      <c r="AQ2" s="7"/>
+      <c r="AR2" s="7"/>
+    </row>
+    <row r="3" spans="1:90" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="D3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="E3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="G3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:89" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="K3" s="6"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7"/>
-      <c r="AD3" s="7"/>
-      <c r="AE3" s="7"/>
-      <c r="AF3" s="7"/>
-      <c r="AG3" s="7"/>
-      <c r="AH3" s="7"/>
-      <c r="AI3" s="7"/>
-      <c r="AJ3" s="7"/>
-      <c r="AK3" s="7"/>
-      <c r="AL3" s="7"/>
-      <c r="AM3" s="7"/>
-      <c r="AN3" s="7"/>
-      <c r="AO3" s="7"/>
-      <c r="AP3" s="7"/>
-      <c r="AQ3" s="7"/>
-    </row>
-    <row r="4" spans="1:89" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
-      <c r="AB4" s="10"/>
-      <c r="AC4" s="10"/>
-      <c r="AD4" s="10"/>
-      <c r="AE4" s="10"/>
-      <c r="AF4" s="10"/>
-      <c r="AG4" s="10"/>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="10"/>
-      <c r="AL4" s="10"/>
-      <c r="AM4" s="10"/>
-      <c r="AN4" s="10"/>
-      <c r="AO4" s="10"/>
-      <c r="AP4" s="10"/>
-      <c r="AQ4" s="10"/>
-      <c r="AR4" s="10"/>
-      <c r="AS4" s="10"/>
-      <c r="AT4" s="10"/>
-      <c r="AU4" s="10"/>
-      <c r="AV4" s="10"/>
-      <c r="AW4" s="10"/>
-      <c r="AX4" s="10"/>
-      <c r="AY4" s="10"/>
-      <c r="AZ4" s="10"/>
-      <c r="BA4" s="10"/>
-      <c r="BB4" s="10"/>
-      <c r="BC4" s="10"/>
-      <c r="BD4" s="10"/>
-      <c r="BE4" s="10"/>
-      <c r="BF4" s="10"/>
-      <c r="BG4" s="10"/>
-      <c r="BH4" s="10"/>
-      <c r="BI4" s="10"/>
-      <c r="BJ4" s="10"/>
-      <c r="BK4" s="10"/>
-      <c r="BL4" s="10"/>
-      <c r="BM4" s="10"/>
-      <c r="BN4" s="10"/>
-      <c r="BO4" s="10"/>
-      <c r="BP4" s="10"/>
-      <c r="BQ4" s="10"/>
-      <c r="BR4" s="10"/>
-      <c r="BS4" s="10"/>
-      <c r="BT4" s="10"/>
-      <c r="BU4" s="10"/>
-      <c r="BV4" s="10"/>
-      <c r="BW4" s="10"/>
-      <c r="BX4" s="10"/>
-      <c r="BY4" s="10"/>
-      <c r="BZ4" s="10"/>
-      <c r="CA4" s="10"/>
-      <c r="CB4" s="10"/>
-      <c r="CC4" s="10"/>
-      <c r="CD4" s="10"/>
-      <c r="CE4" s="10"/>
-      <c r="CF4" s="10"/>
-      <c r="CG4" s="10"/>
-      <c r="CH4" s="10"/>
-      <c r="CI4" s="10"/>
-      <c r="CJ4" s="10"/>
-      <c r="CK4" s="10"/>
-    </row>
-    <row r="5" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
+      <c r="AH3" s="10"/>
+      <c r="AI3" s="10"/>
+      <c r="AJ3" s="10"/>
+      <c r="AK3" s="10"/>
+      <c r="AL3" s="10"/>
+      <c r="AM3" s="10"/>
+      <c r="AN3" s="10"/>
+      <c r="AO3" s="10"/>
+      <c r="AP3" s="10"/>
+      <c r="AQ3" s="10"/>
+      <c r="AR3" s="10"/>
+      <c r="AS3" s="10"/>
+      <c r="AT3" s="10"/>
+      <c r="AU3" s="10"/>
+      <c r="AV3" s="10"/>
+      <c r="AW3" s="10"/>
+      <c r="AX3" s="10"/>
+      <c r="AY3" s="10"/>
+      <c r="AZ3" s="10"/>
+      <c r="BA3" s="10"/>
+      <c r="BB3" s="10"/>
+      <c r="BC3" s="10"/>
+      <c r="BD3" s="10"/>
+      <c r="BE3" s="10"/>
+      <c r="BF3" s="10"/>
+      <c r="BG3" s="10"/>
+      <c r="BH3" s="10"/>
+      <c r="BI3" s="10"/>
+      <c r="BJ3" s="10"/>
+      <c r="BK3" s="10"/>
+      <c r="BL3" s="10"/>
+      <c r="BM3" s="10"/>
+      <c r="BN3" s="10"/>
+      <c r="BO3" s="10"/>
+      <c r="BP3" s="10"/>
+      <c r="BQ3" s="10"/>
+      <c r="BR3" s="10"/>
+      <c r="BS3" s="10"/>
+      <c r="BT3" s="10"/>
+      <c r="BU3" s="10"/>
+      <c r="BV3" s="10"/>
+      <c r="BW3" s="10"/>
+      <c r="BX3" s="10"/>
+      <c r="BY3" s="10"/>
+      <c r="BZ3" s="10"/>
+      <c r="CA3" s="10"/>
+      <c r="CB3" s="10"/>
+      <c r="CC3" s="10"/>
+      <c r="CD3" s="10"/>
+      <c r="CE3" s="10"/>
+      <c r="CF3" s="10"/>
+      <c r="CG3" s="10"/>
+      <c r="CH3" s="10"/>
+      <c r="CI3" s="10"/>
+      <c r="CJ3" s="10"/>
+      <c r="CK3" s="10"/>
+      <c r="CL3" s="10"/>
+    </row>
+    <row r="4" spans="1:90" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="7"/>
+      <c r="AG4" s="7"/>
+      <c r="AH4" s="7"/>
+      <c r="AI4" s="7"/>
+      <c r="AJ4" s="7"/>
+      <c r="AK4" s="7"/>
+      <c r="AL4" s="7"/>
+      <c r="AM4" s="7"/>
+      <c r="AN4" s="7"/>
+      <c r="AO4" s="7"/>
+      <c r="AP4" s="7"/>
+      <c r="AQ4" s="7"/>
+      <c r="AR4" s="7"/>
+    </row>
+    <row r="5" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="17"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="15"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="7"/>
+      <c r="G5" s="17"/>
+      <c r="L5" s="6"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
@@ -761,16 +767,17 @@
       <c r="AO5" s="7"/>
       <c r="AP5" s="7"/>
       <c r="AQ5" s="7"/>
-    </row>
-    <row r="6" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="AR5" s="7"/>
+    </row>
+    <row r="6" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="17"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="15"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="7"/>
+      <c r="G6" s="17"/>
+      <c r="L6" s="6"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
@@ -802,16 +809,17 @@
       <c r="AO6" s="7"/>
       <c r="AP6" s="7"/>
       <c r="AQ6" s="7"/>
-    </row>
-    <row r="7" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="AR6" s="7"/>
+    </row>
+    <row r="7" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="17"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="15"/>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="7"/>
+      <c r="G7" s="17"/>
+      <c r="L7" s="6"/>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
@@ -842,17 +850,16 @@
       <c r="AN7" s="7"/>
       <c r="AO7" s="7"/>
       <c r="AP7" s="7"/>
-      <c r="AQ7" s="7"/>
-    </row>
-    <row r="8" spans="1:89" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="17"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="7"/>
+      <c r="G8" s="17"/>
+      <c r="L8" s="6"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -882,16 +889,17 @@
       <c r="AM8" s="7"/>
       <c r="AN8" s="7"/>
       <c r="AO8" s="7"/>
-    </row>
-    <row r="9" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="AP8" s="7"/>
+    </row>
+    <row r="9" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="17"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="7"/>
+      <c r="G9" s="17"/>
+      <c r="L9" s="6"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
@@ -921,16 +929,17 @@
       <c r="AM9" s="7"/>
       <c r="AN9" s="7"/>
       <c r="AO9" s="7"/>
-    </row>
-    <row r="10" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="AP9" s="7"/>
+    </row>
+    <row r="10" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="17"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="15"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="7"/>
+      <c r="G10" s="17"/>
+      <c r="L10" s="6"/>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
@@ -960,16 +969,17 @@
       <c r="AM10" s="7"/>
       <c r="AN10" s="7"/>
       <c r="AO10" s="7"/>
-    </row>
-    <row r="11" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="AP10" s="7"/>
+    </row>
+    <row r="11" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="17"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="15"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="7"/>
+      <c r="G11" s="17"/>
+      <c r="L11" s="6"/>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
@@ -999,16 +1009,17 @@
       <c r="AM11" s="7"/>
       <c r="AN11" s="7"/>
       <c r="AO11" s="7"/>
-    </row>
-    <row r="12" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="AP11" s="7"/>
+    </row>
+    <row r="12" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="17"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="15"/>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="7"/>
+      <c r="G12" s="17"/>
+      <c r="L12" s="6"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
@@ -1038,49 +1049,11 @@
       <c r="AM12" s="7"/>
       <c r="AN12" s="7"/>
       <c r="AO12" s="7"/>
-    </row>
-    <row r="13" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="7"/>
-      <c r="Z13" s="7"/>
-      <c r="AA13" s="7"/>
-      <c r="AB13" s="7"/>
-      <c r="AC13" s="7"/>
-      <c r="AD13" s="7"/>
-      <c r="AE13" s="7"/>
-      <c r="AF13" s="7"/>
-      <c r="AG13" s="7"/>
-      <c r="AH13" s="7"/>
-      <c r="AI13" s="7"/>
-      <c r="AJ13" s="7"/>
-      <c r="AK13" s="7"/>
-      <c r="AL13" s="7"/>
-      <c r="AM13" s="7"/>
-      <c r="AN13" s="7"/>
-      <c r="AO13" s="7"/>
+      <c r="AP12" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>